<commit_message>
Finishes implementing BFS for table ordering
</commit_message>
<xml_diff>
--- a/METER_DATOS/Nuevos Espacios.xlsx
+++ b/METER_DATOS/Nuevos Espacios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Carlos\Trabajo\Icloud Soft Facility Management\CNXN_MYSQL\METER_DATOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D27064-0563-4B78-AA5A-F1C075471B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F7C113-0309-449F-9AB4-66E903D21FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{48A5FF39-7C89-4E4B-91D8-8A8BD96191FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48A5FF39-7C89-4E4B-91D8-8A8BD96191FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -114,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,14 +124,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -167,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -175,12 +167,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -490,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F0B7B2-784E-4E7D-8CDA-C6B6029BA946}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,15 +817,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I20" s="3"/>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:K9">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{DB00724E-8D8E-4707-A4C9-B51E30CCA824}">
       <formula1>"Floors and Rooms, Rooms Only"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added spaces but not editable
</commit_message>
<xml_diff>
--- a/METER_DATOS/Nuevos Espacios.xlsx
+++ b/METER_DATOS/Nuevos Espacios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Carlos\Trabajo\Icloud Soft Facility Management\CNXN_MYSQL\METER_DATOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F7C113-0309-449F-9AB4-66E903D21FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5C98B7-C194-491D-970C-E387B4C09FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{48A5FF39-7C89-4E4B-91D8-8A8BD96191FF}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{48A5FF39-7C89-4E4B-91D8-8A8BD96191FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
   <si>
     <t>CAMPUS</t>
   </si>
@@ -53,9 +53,6 @@
     <t>EDIFICIO</t>
   </si>
   <si>
-    <t>ESTRUCTURA</t>
-  </si>
-  <si>
     <t>PLANTA</t>
   </si>
   <si>
@@ -65,21 +62,12 @@
     <t>CREADO POR</t>
   </si>
   <si>
-    <t>TIPO EDIFICIO</t>
-  </si>
-  <si>
-    <t>TIPO ESTRUCTURA</t>
-  </si>
-  <si>
     <t>MADRID</t>
   </si>
   <si>
     <t>LAS TABLAS</t>
   </si>
   <si>
-    <t>Floors and Rooms</t>
-  </si>
-  <si>
     <t>ESTANCIA</t>
   </si>
   <si>
@@ -108,13 +96,28 @@
   </si>
   <si>
     <t>OFICINA 2</t>
+  </si>
+  <si>
+    <t>PARQUE</t>
+  </si>
+  <si>
+    <t>Es un parque</t>
+  </si>
+  <si>
+    <t>El hall principal, suelo de mármol</t>
+  </si>
+  <si>
+    <t>ESPACIO</t>
+  </si>
+  <si>
+    <t>AREA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +127,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -159,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -167,6 +178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -491,16 +503,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F0B7B2-784E-4E7D-8CDA-C6B6029BA946}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -511,28 +524,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>1</v>
@@ -540,294 +553,286 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:K9">
+  <conditionalFormatting sqref="A2:K11">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10" xr:uid="{DB00724E-8D8E-4707-A4C9-B51E30CCA824}">
-      <formula1>"Floors and Rooms, Rooms Only"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>